<commit_message>
add express of money
</commit_message>
<xml_diff>
--- a/server/modules/buganalysis/totalBugs.xlsx
+++ b/server/modules/buganalysis/totalBugs.xlsx
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M27"/>
+  <dimension ref="A1:N27"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -420,6 +420,9 @@
       <c r="M1" t="str">
         <v>201911</v>
       </c>
+      <c r="N1" t="str">
+        <v>201912</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
@@ -461,6 +464,9 @@
       <c r="M2">
         <v>0</v>
       </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
@@ -502,6 +508,9 @@
       <c r="M3">
         <v>9</v>
       </c>
+      <c r="N3">
+        <v>0</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
@@ -543,6 +552,9 @@
       <c r="M4">
         <v>8</v>
       </c>
+      <c r="N4">
+        <v>2</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
@@ -566,6 +578,9 @@
       <c r="M5">
         <v>1</v>
       </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
@@ -601,6 +616,9 @@
       <c r="M6">
         <v>4</v>
       </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
@@ -629,6 +647,9 @@
       <c r="M8">
         <v>0</v>
       </c>
+      <c r="N8">
+        <v>1</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="str">
@@ -646,6 +667,9 @@
       <c r="M9">
         <v>1</v>
       </c>
+      <c r="N9">
+        <v>4</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="str">
@@ -663,6 +687,9 @@
       <c r="M10">
         <v>0</v>
       </c>
+      <c r="N10">
+        <v>0</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="str">
@@ -674,6 +701,9 @@
       <c r="M11">
         <v>2</v>
       </c>
+      <c r="N11">
+        <v>2</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="str">
@@ -715,6 +745,9 @@
       <c r="M12">
         <v>1</v>
       </c>
+      <c r="N12">
+        <v>2</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="str">
@@ -756,6 +789,9 @@
       <c r="M13">
         <v>9</v>
       </c>
+      <c r="N13">
+        <v>1</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="str">
@@ -773,6 +809,9 @@
       <c r="M14">
         <v>5</v>
       </c>
+      <c r="N14">
+        <v>1</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="str">
@@ -814,6 +853,9 @@
       <c r="M15">
         <v>0</v>
       </c>
+      <c r="N15">
+        <v>1</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="str">
@@ -855,6 +897,9 @@
       <c r="M16">
         <v>7</v>
       </c>
+      <c r="N16">
+        <v>3</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="str">
@@ -890,6 +935,9 @@
       <c r="M17">
         <v>1</v>
       </c>
+      <c r="N17">
+        <v>0</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="str">
@@ -919,6 +967,9 @@
       <c r="M18">
         <v>1</v>
       </c>
+      <c r="N18">
+        <v>0</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="str">
@@ -933,6 +984,9 @@
       <c r="M19">
         <v>0</v>
       </c>
+      <c r="N19">
+        <v>0</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="str">
@@ -944,6 +998,9 @@
       <c r="M20">
         <v>0</v>
       </c>
+      <c r="N20">
+        <v>0</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="str">
@@ -985,6 +1042,9 @@
       <c r="M21">
         <v>6</v>
       </c>
+      <c r="N21">
+        <v>1</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="str">
@@ -1026,6 +1086,9 @@
       <c r="M22">
         <v>2</v>
       </c>
+      <c r="N22">
+        <v>1</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="str">
@@ -1046,6 +1109,9 @@
       <c r="M23">
         <v>3</v>
       </c>
+      <c r="N23">
+        <v>0</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="str">
@@ -1087,6 +1153,9 @@
       <c r="M24">
         <v>6</v>
       </c>
+      <c r="N24">
+        <v>0</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="str">
@@ -1104,6 +1173,9 @@
       <c r="M25">
         <v>2</v>
       </c>
+      <c r="N25">
+        <v>0</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="str">
@@ -1126,10 +1198,13 @@
       <c r="M27">
         <v>3</v>
       </c>
+      <c r="N27">
+        <v>3</v>
+      </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:M27"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:N27"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>